<commit_message>
EPBDS Fix for TBasicRuntimeEnv delegator to enable RuntimeContext modifications.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/engine/TestContextManaginFromRules.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/engine/TestContextManaginFromRules.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CurretContextTest" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="69">
   <si>
     <t>C1</t>
   </si>
@@ -193,13 +193,46 @@
   </si>
   <si>
     <t>return checkInitialContextContext();</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Operation Execution</t>
+  </si>
+  <si>
+    <t>EXIT</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>setContextTest()</t>
+  </si>
+  <si>
+    <t>Algorithm boolean tbasicCaller()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,8 +280,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color indexed="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +387,80 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor theme="5" tint="0.39994506668294322"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="29"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC66"/>
+        <bgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="25"/>
+        <bgColor indexed="61"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="50"/>
+        <bgColor indexed="51"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+        <bgColor indexed="49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="29"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="53"/>
+        <bgColor indexed="29"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="13"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -476,11 +608,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="9"/>
+      </left>
+      <right style="medium">
+        <color indexed="9"/>
+      </right>
+      <top style="medium">
+        <color indexed="9"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="9"/>
+      </left>
+      <right style="medium">
+        <color indexed="9"/>
+      </right>
+      <top style="medium">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="9"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="9"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="9"/>
+      </left>
+      <right style="medium">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -503,6 +707,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -546,9 +753,45 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,7 +1088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C6:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -854,40 +1099,40 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:4">
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="30"/>
     </row>
     <row r="7" spans="3:4">
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="32"/>
     </row>
     <row r="8" spans="3:4">
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="21"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="9" spans="3:4">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="3:4">
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="28"/>
     </row>
     <row r="11" spans="3:4">
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -948,63 +1193,63 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="34"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="28"/>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="28"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="6" t="s">
@@ -1084,9 +1329,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D20"/>
+  <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1095,55 +1342,116 @@
     <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1">
+    <row r="2" spans="2:10" ht="21" thickBot="1">
+      <c r="F2" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+    </row>
+    <row r="3" spans="2:10" ht="21.75" thickBot="1">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="35" t="s">
+      <c r="F3" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="21.75" thickBot="1">
+      <c r="B4" s="20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" s="8" customFormat="1">
-      <c r="B5" s="36" t="s">
+      <c r="F4" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="48"/>
+    </row>
+    <row r="5" spans="2:10" s="8" customFormat="1" ht="21">
+      <c r="B5" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" s="8" customFormat="1">
-      <c r="B6" s="36" t="s">
+      <c r="F5" s="49"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" s="8" customFormat="1" ht="15.75">
+      <c r="B6" s="21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" s="8" customFormat="1">
-      <c r="B7" s="36" t="s">
+      <c r="F6" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="56"/>
+    </row>
+    <row r="7" spans="2:10" s="8" customFormat="1">
+      <c r="B7" s="21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B8" s="37" t="s">
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B8" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:10">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:10">
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="26" t="s">
+    <row r="14" spans="2:10">
+      <c r="B14" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-    </row>
-    <row r="15" spans="2:4">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" spans="2:10">
       <c r="B15" s="7" t="s">
         <v>0</v>
       </c>
@@ -1154,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:10">
       <c r="B16" s="4" t="s">
         <v>21</v>
       </c>
@@ -1206,8 +1514,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1236,65 +1549,65 @@
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
     </row>
     <row r="8" spans="2:4" s="19" customFormat="1">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:4" s="19" customFormat="1">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="2:4" s="19" customFormat="1">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="21" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="2:4" s="19" customFormat="1">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="21" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:4" s="19" customFormat="1">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:4" s="19" customFormat="1">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="21" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:4" s="19" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="22" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1324,11 +1637,11 @@
       <c r="D19" s="19"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="18" t="s">
@@ -1393,12 +1706,12 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="18" t="s">
@@ -1479,11 +1792,11 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="18" t="s">
@@ -1576,10 +1889,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="37"/>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" s="9" t="s">

</xml_diff>